<commit_message>
completed all scenarios we can, just waiting on the summer low flow d & v .tifs for Pahsimeroi
</commit_message>
<xml_diff>
--- a/analysis/scenarios_to_run.xlsx
+++ b/analysis/scenarios_to_run.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABEACE02EC0C739979305ADE589C" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{1EDF86F5-BEC4-4EB4-A936-87524579EB29}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="11_F25DC773A252ABEACE02EC0C739979305ADE589C" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D79CFDE5-3A2F-474A-84F5-1AC6E97637B1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="32">
   <si>
     <t>Watershed</t>
   </si>
@@ -151,13 +151,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,10 +445,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B2:I22"/>
+  <dimension ref="B2:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,7 +463,7 @@
     <col min="9" max="9" width="15.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>13</v>
       </c>
@@ -486,7 +489,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -508,8 +511,11 @@
       <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I3" s="2">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -531,8 +537,11 @@
       <c r="H4" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I4" s="2">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -554,8 +563,11 @@
       <c r="H5" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I5" s="2">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -577,8 +589,11 @@
       <c r="H6" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="2">
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -600,8 +615,11 @@
       <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I7" s="2">
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -623,8 +641,11 @@
       <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I8" s="2">
+        <v>43861</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -640,14 +661,8 @@
       <c r="F9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -664,13 +679,18 @@
         <v>10</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I10" s="2">
+        <v>43860</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -681,19 +701,23 @@
         <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="I11" s="2">
+        <v>43860</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -701,10 +725,10 @@
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
@@ -715,8 +739,11 @@
       <c r="H12" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="2">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -730,16 +757,11 @@
         <v>7</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -750,68 +772,73 @@
         <v>6</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="I14" s="2">
+        <v>43860</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I15" s="2">
-        <v>43859</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+        <v>43861</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="I16" s="2">
-        <v>43859</v>
+        <v>43861</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
@@ -828,13 +855,13 @@
         <v>7</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I17" s="2">
         <v>43859</v>
@@ -851,16 +878,16 @@
         <v>5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I18" s="2">
         <v>43859</v>
@@ -874,22 +901,22 @@
         <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I19" s="2">
-        <v>43860</v>
+        <v>43859</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
@@ -900,22 +927,22 @@
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I20" s="2">
-        <v>43860</v>
+        <v>43859</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
@@ -932,13 +959,13 @@
         <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I21" s="2">
         <v>43860</v>
@@ -955,16 +982,71 @@
         <v>6</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="2">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>21</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="2">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>30</v>
+      </c>
+      <c r="I24" s="2">
+        <v>43860</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +1068,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D644EA8E-A834-4F66-8CAA-8928B8178A2C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DA032E8-BA59-4AF0-B2EF-520F19C91F1B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>